<commit_message>
unique day graphs using plotly
</commit_message>
<xml_diff>
--- a/Workout 2026.xlsx
+++ b/Workout 2026.xlsx
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Squats</t>
-  </si>
-  <si>
-    <t>Relax - Stretch - Yoga</t>
   </si>
   <si>
     <t>Deadlift</t>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>No Abs</t>
+  </si>
+  <si>
+    <t>Relax - Stretch - Yoga</t>
   </si>
   <si>
     <t>Figure 8 - 30 sec</t>
@@ -820,11 +820,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="368328398"/>
-        <c:axId val="1869734787"/>
+        <c:axId val="1086881834"/>
+        <c:axId val="1927338576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="368328398"/>
+        <c:axId val="1086881834"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,10 +876,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1869734787"/>
+        <c:crossAx val="1927338576"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1869734787"/>
+        <c:axId val="1927338576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -955,7 +955,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368328398"/>
+        <c:crossAx val="1086881834"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1058,11 +1058,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1543809503"/>
-        <c:axId val="576570283"/>
+        <c:axId val="1311146052"/>
+        <c:axId val="1774563847"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1543809503"/>
+        <c:axId val="1311146052"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,10 +1114,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="576570283"/>
+        <c:crossAx val="1774563847"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="576570283"/>
+        <c:axId val="1774563847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1193,7 +1193,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1543809503"/>
+        <c:crossAx val="1311146052"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1296,11 +1296,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2039137545"/>
-        <c:axId val="790382214"/>
+        <c:axId val="2058528156"/>
+        <c:axId val="999440508"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2039137545"/>
+        <c:axId val="2058528156"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,10 +1352,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="790382214"/>
+        <c:crossAx val="999440508"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="790382214"/>
+        <c:axId val="999440508"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1431,7 +1431,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2039137545"/>
+        <c:crossAx val="2058528156"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1534,11 +1534,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2082938734"/>
-        <c:axId val="789306345"/>
+        <c:axId val="1720321586"/>
+        <c:axId val="371479548"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2082938734"/>
+        <c:axId val="1720321586"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1590,10 +1590,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="789306345"/>
+        <c:crossAx val="371479548"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="789306345"/>
+        <c:axId val="371479548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1669,7 +1669,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2082938734"/>
+        <c:crossAx val="1720321586"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1772,11 +1772,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1462896721"/>
-        <c:axId val="175175079"/>
+        <c:axId val="1781695587"/>
+        <c:axId val="326480498"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1462896721"/>
+        <c:axId val="1781695587"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,10 +1828,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175175079"/>
+        <c:crossAx val="326480498"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175175079"/>
+        <c:axId val="326480498"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1907,7 +1907,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1462896721"/>
+        <c:crossAx val="1781695587"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2010,11 +2010,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="281838614"/>
-        <c:axId val="708083950"/>
+        <c:axId val="1498124136"/>
+        <c:axId val="92694270"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="281838614"/>
+        <c:axId val="1498124136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2066,10 +2066,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708083950"/>
+        <c:crossAx val="92694270"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="708083950"/>
+        <c:axId val="92694270"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2145,7 +2145,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281838614"/>
+        <c:crossAx val="1498124136"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2248,11 +2248,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1058277716"/>
-        <c:axId val="987398654"/>
+        <c:axId val="1518747131"/>
+        <c:axId val="1372551975"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1058277716"/>
+        <c:axId val="1518747131"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2304,10 +2304,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="987398654"/>
+        <c:crossAx val="1372551975"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="987398654"/>
+        <c:axId val="1372551975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2383,7 +2383,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1058277716"/>
+        <c:crossAx val="1518747131"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2486,11 +2486,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="78364419"/>
-        <c:axId val="188136247"/>
+        <c:axId val="61472078"/>
+        <c:axId val="457380372"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78364419"/>
+        <c:axId val="61472078"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2542,10 +2542,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188136247"/>
+        <c:crossAx val="457380372"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188136247"/>
+        <c:axId val="457380372"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2621,7 +2621,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78364419"/>
+        <c:crossAx val="61472078"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2724,11 +2724,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="945866661"/>
-        <c:axId val="1300523481"/>
+        <c:axId val="1700920040"/>
+        <c:axId val="24946193"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="945866661"/>
+        <c:axId val="1700920040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2780,10 +2780,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1300523481"/>
+        <c:crossAx val="24946193"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1300523481"/>
+        <c:axId val="24946193"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2859,7 +2859,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="945866661"/>
+        <c:crossAx val="1700920040"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2962,11 +2962,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2084227382"/>
-        <c:axId val="635512212"/>
+        <c:axId val="1323156742"/>
+        <c:axId val="294683485"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2084227382"/>
+        <c:axId val="1323156742"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3018,10 +3018,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="635512212"/>
+        <c:crossAx val="294683485"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="635512212"/>
+        <c:axId val="294683485"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3097,7 +3097,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084227382"/>
+        <c:crossAx val="1323156742"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3200,11 +3200,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1248506682"/>
-        <c:axId val="1515481738"/>
+        <c:axId val="1058286828"/>
+        <c:axId val="101734466"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1248506682"/>
+        <c:axId val="1058286828"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3256,10 +3256,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1515481738"/>
+        <c:crossAx val="101734466"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1515481738"/>
+        <c:axId val="101734466"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3335,7 +3335,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1248506682"/>
+        <c:crossAx val="1058286828"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3438,11 +3438,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="103145621"/>
-        <c:axId val="1012405935"/>
+        <c:axId val="1028837646"/>
+        <c:axId val="1210893258"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103145621"/>
+        <c:axId val="1028837646"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3494,10 +3494,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1012405935"/>
+        <c:crossAx val="1210893258"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1012405935"/>
+        <c:axId val="1210893258"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3573,7 +3573,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103145621"/>
+        <c:crossAx val="1028837646"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3676,11 +3676,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="451323225"/>
-        <c:axId val="616633389"/>
+        <c:axId val="1263509863"/>
+        <c:axId val="1060887814"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="451323225"/>
+        <c:axId val="1263509863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3732,10 +3732,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="616633389"/>
+        <c:crossAx val="1060887814"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="616633389"/>
+        <c:axId val="1060887814"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3811,7 +3811,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451323225"/>
+        <c:crossAx val="1263509863"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3914,11 +3914,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2071670447"/>
-        <c:axId val="1963158563"/>
+        <c:axId val="582046756"/>
+        <c:axId val="1792929499"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2071670447"/>
+        <c:axId val="582046756"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,10 +3970,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963158563"/>
+        <c:crossAx val="1792929499"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1963158563"/>
+        <c:axId val="1792929499"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4049,7 +4049,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2071670447"/>
+        <c:crossAx val="582046756"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4152,11 +4152,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="182560964"/>
-        <c:axId val="1020394635"/>
+        <c:axId val="252701318"/>
+        <c:axId val="1058513719"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182560964"/>
+        <c:axId val="252701318"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4208,10 +4208,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1020394635"/>
+        <c:crossAx val="1058513719"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1020394635"/>
+        <c:axId val="1058513719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4287,7 +4287,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182560964"/>
+        <c:crossAx val="252701318"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4390,11 +4390,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1641522680"/>
-        <c:axId val="2119318070"/>
+        <c:axId val="1736465629"/>
+        <c:axId val="994546289"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1641522680"/>
+        <c:axId val="1736465629"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4446,10 +4446,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119318070"/>
+        <c:crossAx val="994546289"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119318070"/>
+        <c:axId val="994546289"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4525,7 +4525,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1641522680"/>
+        <c:crossAx val="1736465629"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4628,11 +4628,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="946291377"/>
-        <c:axId val="1046233187"/>
+        <c:axId val="1593000190"/>
+        <c:axId val="1804590746"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="946291377"/>
+        <c:axId val="1593000190"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4684,10 +4684,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1046233187"/>
+        <c:crossAx val="1804590746"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1046233187"/>
+        <c:axId val="1804590746"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4763,7 +4763,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="946291377"/>
+        <c:crossAx val="1593000190"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4866,11 +4866,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="733883906"/>
-        <c:axId val="543697049"/>
+        <c:axId val="427661687"/>
+        <c:axId val="375649840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="733883906"/>
+        <c:axId val="427661687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4922,10 +4922,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543697049"/>
+        <c:crossAx val="375649840"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="543697049"/>
+        <c:axId val="375649840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -5001,7 +5001,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="733883906"/>
+        <c:crossAx val="427661687"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5104,11 +5104,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1677347837"/>
-        <c:axId val="646129329"/>
+        <c:axId val="947329759"/>
+        <c:axId val="1128599213"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1677347837"/>
+        <c:axId val="947329759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5160,10 +5160,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="646129329"/>
+        <c:crossAx val="1128599213"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="646129329"/>
+        <c:axId val="1128599213"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -5239,7 +5239,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1677347837"/>
+        <c:crossAx val="947329759"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5342,11 +5342,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1277435042"/>
-        <c:axId val="1959886023"/>
+        <c:axId val="377063374"/>
+        <c:axId val="397459589"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1277435042"/>
+        <c:axId val="377063374"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5398,10 +5398,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1959886023"/>
+        <c:crossAx val="397459589"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1959886023"/>
+        <c:axId val="397459589"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -5477,7 +5477,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277435042"/>
+        <c:crossAx val="377063374"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5580,11 +5580,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97878084"/>
-        <c:axId val="254079249"/>
+        <c:axId val="343976863"/>
+        <c:axId val="350108890"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97878084"/>
+        <c:axId val="343976863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5636,10 +5636,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254079249"/>
+        <c:crossAx val="350108890"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254079249"/>
+        <c:axId val="350108890"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -5715,7 +5715,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97878084"/>
+        <c:crossAx val="343976863"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5818,11 +5818,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="893854082"/>
-        <c:axId val="316143728"/>
+        <c:axId val="668175608"/>
+        <c:axId val="1468978232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="893854082"/>
+        <c:axId val="668175608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5874,10 +5874,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316143728"/>
+        <c:crossAx val="1468978232"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316143728"/>
+        <c:axId val="1468978232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -5953,7 +5953,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="893854082"/>
+        <c:crossAx val="668175608"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6056,11 +6056,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1850360716"/>
-        <c:axId val="52624800"/>
+        <c:axId val="1296091857"/>
+        <c:axId val="101186668"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1850360716"/>
+        <c:axId val="1296091857"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6112,10 +6112,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52624800"/>
+        <c:crossAx val="101186668"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52624800"/>
+        <c:axId val="101186668"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -6191,7 +6191,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1850360716"/>
+        <c:crossAx val="1296091857"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6294,11 +6294,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1896921347"/>
-        <c:axId val="1155283945"/>
+        <c:axId val="737228209"/>
+        <c:axId val="1099916511"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1896921347"/>
+        <c:axId val="737228209"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6350,10 +6350,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1155283945"/>
+        <c:crossAx val="1099916511"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1155283945"/>
+        <c:axId val="1099916511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -6429,7 +6429,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1896921347"/>
+        <c:crossAx val="737228209"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -7008,9 +7008,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="8086725" cy="5000625"/>
     <xdr:graphicFrame>
@@ -7457,111 +7457,111 @@
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D4" s="6"/>
       <c r="F4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="G6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="C8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="E8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>37</v>
-      </c>
       <c r="G8" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -7812,7 +7812,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -7837,7 +7837,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -7862,7 +7862,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -7887,7 +7887,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -7912,7 +7912,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -7937,7 +7937,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -7971,7 +7971,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -7996,7 +7996,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -8021,7 +8021,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -8046,7 +8046,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -8071,7 +8071,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -8096,7 +8096,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -8121,7 +8121,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -8146,7 +8146,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -8171,7 +8171,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -8196,7 +8196,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -8286,7 +8286,7 @@
     </row>
     <row r="2">
       <c r="A2" s="43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="44">
@@ -8311,7 +8311,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -8336,7 +8336,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -8361,7 +8361,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -8386,7 +8386,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -8411,7 +8411,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -8445,7 +8445,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -8470,7 +8470,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -8495,7 +8495,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -8520,7 +8520,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -8545,7 +8545,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -8570,7 +8570,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -8595,7 +8595,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -8620,7 +8620,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -8645,7 +8645,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -8670,7 +8670,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -8760,7 +8760,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -8785,7 +8785,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -8810,7 +8810,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -8835,7 +8835,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -8860,7 +8860,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -8885,7 +8885,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -8919,7 +8919,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -8944,7 +8944,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -8969,7 +8969,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -8994,7 +8994,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -9019,7 +9019,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -9044,7 +9044,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -9069,7 +9069,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -9094,7 +9094,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -9119,7 +9119,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -9144,7 +9144,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -9234,7 +9234,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>59</v>
@@ -9261,7 +9261,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -9286,7 +9286,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -9311,7 +9311,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -9336,7 +9336,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -9361,7 +9361,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -9395,7 +9395,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -9420,7 +9420,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -9445,7 +9445,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -9470,7 +9470,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -9495,7 +9495,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -9520,7 +9520,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -9545,7 +9545,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -9570,7 +9570,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -9595,7 +9595,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -9620,7 +9620,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -9710,7 +9710,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>59</v>
@@ -9737,7 +9737,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -9762,7 +9762,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -9787,7 +9787,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -9812,7 +9812,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -9837,7 +9837,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -9871,7 +9871,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -9896,7 +9896,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -9921,7 +9921,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -9946,7 +9946,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -9971,7 +9971,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -9996,7 +9996,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -10021,7 +10021,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -10046,7 +10046,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -10071,7 +10071,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -10096,7 +10096,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -11134,7 +11134,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>63</v>
@@ -11161,7 +11161,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>64</v>
@@ -11188,7 +11188,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -11213,7 +11213,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -11238,7 +11238,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -11263,7 +11263,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -11297,7 +11297,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -11322,7 +11322,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -11347,7 +11347,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -11372,7 +11372,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -11397,7 +11397,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -11422,7 +11422,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -11447,7 +11447,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -11481,7 +11481,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -11506,7 +11506,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -11531,7 +11531,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -11610,7 +11610,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>62</v>
@@ -11637,7 +11637,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -11662,7 +11662,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -11687,7 +11687,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -11712,7 +11712,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -11737,7 +11737,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -11771,7 +11771,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -11796,7 +11796,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -11821,7 +11821,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -11846,7 +11846,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -11871,7 +11871,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -11896,7 +11896,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -11921,7 +11921,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -11946,7 +11946,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -11971,7 +11971,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -11996,7 +11996,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -12086,7 +12086,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>65</v>
@@ -12113,7 +12113,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>66</v>
@@ -12140,7 +12140,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -12165,7 +12165,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -12190,7 +12190,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -12215,7 +12215,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -12249,7 +12249,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -12274,7 +12274,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -12299,7 +12299,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -12324,7 +12324,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -12349,7 +12349,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -12374,7 +12374,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -12399,7 +12399,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -12424,7 +12424,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -12449,7 +12449,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -12474,7 +12474,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -12564,7 +12564,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>53</v>
@@ -12591,7 +12591,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -12616,7 +12616,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -12641,7 +12641,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -12666,7 +12666,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -12691,7 +12691,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -12725,7 +12725,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -12750,7 +12750,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -12775,7 +12775,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -12800,7 +12800,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -12825,7 +12825,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -12850,7 +12850,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -12875,7 +12875,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -12900,7 +12900,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -12925,7 +12925,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -12950,7 +12950,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -13027,7 +13027,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -13052,7 +13052,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -13077,7 +13077,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -13102,7 +13102,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -13127,7 +13127,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -13152,7 +13152,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -13186,7 +13186,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -13211,7 +13211,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -13236,7 +13236,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -13261,7 +13261,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -13286,7 +13286,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -13311,7 +13311,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -13336,7 +13336,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -13361,7 +13361,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -13386,7 +13386,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -13411,7 +13411,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -13501,7 +13501,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>67</v>
@@ -13528,7 +13528,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -13553,7 +13553,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -13578,7 +13578,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -13603,7 +13603,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -13628,7 +13628,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -13662,7 +13662,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -13687,7 +13687,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -13712,7 +13712,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -13737,7 +13737,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -13762,7 +13762,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -13787,7 +13787,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -13812,7 +13812,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -13837,7 +13837,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -13862,7 +13862,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -13896,7 +13896,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -13975,7 +13975,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>68</v>
@@ -14002,7 +14002,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -14027,7 +14027,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -14052,7 +14052,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -14077,7 +14077,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -14102,7 +14102,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -14136,7 +14136,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -14161,7 +14161,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -14186,7 +14186,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -14211,7 +14211,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -14236,7 +14236,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -14270,7 +14270,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -14295,7 +14295,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -14320,7 +14320,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -14345,7 +14345,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -14370,7 +14370,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -14923,7 +14923,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>53</v>
@@ -14950,7 +14950,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -14975,7 +14975,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -15000,7 +15000,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -15025,7 +15025,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -15050,7 +15050,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -15084,7 +15084,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -15109,7 +15109,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -15134,7 +15134,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -15159,7 +15159,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -15184,7 +15184,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -15209,7 +15209,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -15234,7 +15234,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -15259,7 +15259,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -15284,7 +15284,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -15309,7 +15309,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -15399,7 +15399,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>70</v>
@@ -15426,7 +15426,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -15451,7 +15451,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -15476,7 +15476,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -15501,7 +15501,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -15526,7 +15526,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -15551,7 +15551,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -15585,7 +15585,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -15610,7 +15610,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -15635,7 +15635,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -15660,7 +15660,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -15685,7 +15685,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -15710,7 +15710,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -15735,7 +15735,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -15760,7 +15760,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -15785,7 +15785,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -15847,7 +15847,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
@@ -15949,7 +15949,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -15973,7 +15973,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -15997,7 +15997,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -16021,7 +16021,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -16045,7 +16045,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -16069,7 +16069,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -16102,7 +16102,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -16126,7 +16126,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -16150,7 +16150,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -16174,7 +16174,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -16198,7 +16198,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -16222,7 +16222,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -16246,7 +16246,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -16270,7 +16270,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -16294,7 +16294,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -16318,7 +16318,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -16858,7 +16858,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -16883,7 +16883,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -16908,7 +16908,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -16933,7 +16933,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -16958,7 +16958,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -16983,7 +16983,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -17017,7 +17017,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -17042,7 +17042,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -17067,7 +17067,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -17092,7 +17092,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -17117,7 +17117,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -17142,7 +17142,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -17167,7 +17167,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -17192,7 +17192,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -17217,7 +17217,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -17242,7 +17242,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -17806,7 +17806,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -17831,7 +17831,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -17856,7 +17856,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -17881,7 +17881,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -17906,7 +17906,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -17931,7 +17931,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -17965,7 +17965,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -17990,7 +17990,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -18015,7 +18015,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -18040,7 +18040,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -18065,7 +18065,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -18090,7 +18090,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -18115,7 +18115,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -18140,7 +18140,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -18165,7 +18165,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -18190,7 +18190,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -18280,7 +18280,7 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -18305,7 +18305,7 @@
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -18330,7 +18330,7 @@
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -18355,7 +18355,7 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -18380,7 +18380,7 @@
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -18405,7 +18405,7 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -18439,7 +18439,7 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -18464,7 +18464,7 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -18489,7 +18489,7 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -18514,7 +18514,7 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -18539,7 +18539,7 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -18564,7 +18564,7 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -18589,7 +18589,7 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -18614,7 +18614,7 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -18639,7 +18639,7 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -18664,7 +18664,7 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">

</xml_diff>